<commit_message>
Docs - docs for KX224 v2.0 Update
</commit_message>
<xml_diff>
--- a/PCB/DOC_LABO/liste_composants_AIS3624.xlsx
+++ b/PCB/DOC_LABO/liste_composants_AIS3624.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Nom de la carte</t>
   </si>
@@ -75,15 +75,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>CMS_805</t>
-  </si>
-  <si>
-    <t>CMS_603 100nF</t>
-  </si>
-  <si>
-    <t>CMS_603_10uF</t>
-  </si>
-  <si>
     <t>Total:</t>
   </si>
   <si>
@@ -91,6 +82,21 @@
   </si>
   <si>
     <t>ACC1</t>
+  </si>
+  <si>
+    <t>Pitch 2,54</t>
+  </si>
+  <si>
+    <t>ADXL355</t>
+  </si>
+  <si>
+    <t>CMS_0805</t>
+  </si>
+  <si>
+    <t>CMS_0603 100nF</t>
+  </si>
+  <si>
+    <t>CMS_0603 10uF</t>
   </si>
 </sst>
 </file>
@@ -481,7 +487,7 @@
   <dimension ref="B3:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,24 +559,28 @@
         <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2">
         <v>1</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2">
         <v>1</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
@@ -583,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -597,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -609,12 +619,12 @@
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" s="5">
         <f>SUM(D11:D15)</f>

</xml_diff>